<commit_message>
Unit Processes for paper - wood and pulp
calc and var files and verified
</commit_message>
<xml_diff>
--- a/data/unitlibrary.xlsx
+++ b/data/unitlibrary.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F34455-7098-EE4E-93D0-B77658320324}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="25200" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="405" yWindow="465" windowWidth="25200" windowHeight="17265"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Processes" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="240">
   <si>
     <t>product</t>
   </si>
@@ -707,12 +706,45 @@
   </si>
   <si>
     <t>Cement Use</t>
+  </si>
+  <si>
+    <t>paper_chipping</t>
+  </si>
+  <si>
+    <t>paper</t>
+  </si>
+  <si>
+    <t>Wood Handling</t>
+  </si>
+  <si>
+    <t>chips</t>
+  </si>
+  <si>
+    <t>data/paper/paper_var.xlsx</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>data/paper/paper_calc.xlsx</t>
+  </si>
+  <si>
+    <t>paper_pulping</t>
+  </si>
+  <si>
+    <t>Pulp Preparation</t>
+  </si>
+  <si>
+    <t>unbleached pulp</t>
+  </si>
+  <si>
+    <t>Pulp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1555,24 +1587,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L55" sqref="L55"/>
+      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7.375" customWidth="1"/>
+    <col min="6" max="6" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1604,7 +1636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -1634,7 +1666,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1664,7 +1696,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -1694,7 +1726,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1724,7 +1756,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1754,7 +1786,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -1784,7 +1816,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -1816,7 +1848,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
@@ -1845,7 +1877,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>74</v>
       </c>
@@ -1874,7 +1906,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
@@ -1903,7 +1935,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
@@ -1932,7 +1964,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
@@ -1961,7 +1993,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -1990,7 +2022,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>67</v>
       </c>
@@ -2019,7 +2051,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
@@ -2048,7 +2080,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>105</v>
       </c>
@@ -2077,7 +2109,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>106</v>
       </c>
@@ -2106,7 +2138,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>80</v>
       </c>
@@ -2135,7 +2167,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>137</v>
       </c>
@@ -2164,7 +2196,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>87</v>
       </c>
@@ -2193,7 +2225,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>91</v>
       </c>
@@ -2222,7 +2254,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>92</v>
       </c>
@@ -2251,7 +2283,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>93</v>
       </c>
@@ -2280,7 +2312,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>112</v>
       </c>
@@ -2309,7 +2341,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>111</v>
       </c>
@@ -2338,7 +2370,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>113</v>
       </c>
@@ -2367,7 +2399,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>118</v>
       </c>
@@ -2396,7 +2428,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>132</v>
       </c>
@@ -2425,7 +2457,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>130</v>
       </c>
@@ -2454,7 +2486,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>140</v>
       </c>
@@ -2483,7 +2515,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>144</v>
       </c>
@@ -2512,7 +2544,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>145</v>
       </c>
@@ -2541,7 +2573,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>146</v>
       </c>
@@ -2570,7 +2602,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>147</v>
       </c>
@@ -2599,7 +2631,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>148</v>
       </c>
@@ -2628,7 +2660,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>149</v>
       </c>
@@ -2657,7 +2689,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>150</v>
       </c>
@@ -2686,7 +2718,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>151</v>
       </c>
@@ -2715,7 +2747,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>169</v>
       </c>
@@ -2744,7 +2776,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>165</v>
       </c>
@@ -2773,7 +2805,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>194</v>
       </c>
@@ -2802,7 +2834,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>191</v>
       </c>
@@ -2831,7 +2863,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>166</v>
       </c>
@@ -2860,7 +2892,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>172</v>
       </c>
@@ -2889,7 +2921,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>175</v>
       </c>
@@ -2918,7 +2950,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>176</v>
       </c>
@@ -2947,7 +2979,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>177</v>
       </c>
@@ -2976,7 +3008,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>187</v>
       </c>
@@ -3005,7 +3037,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>198</v>
       </c>
@@ -3034,7 +3066,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>196</v>
       </c>
@@ -3063,7 +3095,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>197</v>
       </c>
@@ -3092,7 +3124,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>199</v>
       </c>
@@ -3121,7 +3153,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>200</v>
       </c>
@@ -3150,7 +3182,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>201</v>
       </c>
@@ -3179,7 +3211,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>221</v>
       </c>
@@ -3208,7 +3240,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>227</v>
       </c>
@@ -3237,7 +3269,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>226</v>
       </c>
@@ -3264,6 +3296,64 @@
       </c>
       <c r="I58" s="1" t="s">
         <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B59" t="s">
+        <v>230</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B60" t="s">
+        <v>230</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D60" t="s">
+        <v>238</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initalize ethanol unit process data
</commit_message>
<xml_diff>
--- a/data/unitlibrary.xlsx
+++ b/data/unitlibrary.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0853F4DA-3FA4-7049-83BD-2A53B01C23E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF36ACE-1014-A647-8F3A-A111816073C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="460" windowWidth="25200" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8980" yWindow="460" windowWidth="25200" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Processes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="236">
   <si>
     <t>product</t>
   </si>
@@ -706,6 +708,36 @@
   </si>
   <si>
     <t>Power Aux</t>
+  </si>
+  <si>
+    <t>eth_box</t>
+  </si>
+  <si>
+    <t>eth_stoich</t>
+  </si>
+  <si>
+    <t>chemicals</t>
+  </si>
+  <si>
+    <t>C2H6O</t>
+  </si>
+  <si>
+    <t>Ethanol (Black Box)</t>
+  </si>
+  <si>
+    <t>Ethanol (Stoichiometric)</t>
+  </si>
+  <si>
+    <t>data/chemicals/chemvar.xlsx</t>
+  </si>
+  <si>
+    <t>eth-stoich</t>
+  </si>
+  <si>
+    <t>eth-box</t>
+  </si>
+  <si>
+    <t>data/chemicals/chemcals.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1566,13 +1598,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomRight" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3160,6 +3192,64 @@
         <v>220</v>
       </c>
     </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B55" t="s">
+        <v>228</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D55" t="s">
+        <v>229</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B56" t="s">
+        <v>228</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D56" t="s">
+        <v>229</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>